<commit_message>
box plots for completion time
</commit_message>
<xml_diff>
--- a/Results/userStudy.xlsx
+++ b/Results/userStudy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Participant Id</t>
   </si>
@@ -45,6 +45,54 @@
   </si>
   <si>
     <t>non-native</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Median - Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median     </t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Q1 - Min</t>
+  </si>
+  <si>
+    <t>Q3 - Median</t>
+  </si>
+  <si>
+    <t>Max - Q3</t>
+  </si>
+  <si>
+    <t>IQ Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IQ Range </t>
+  </si>
+  <si>
+    <t>IQ * 1.5</t>
+  </si>
+  <si>
+    <t>upper limit threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>up lim thresh - Q3</t>
+  </si>
+  <si>
+    <t>low lim threshold</t>
   </si>
 </sst>
 </file>
@@ -97,6 +145,1139 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Completion Time  for Sorting Task</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(Sheet1!$G$36,Sheet1!$C$36)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>11.5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>Non-assisted</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v> assisted</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$46:$G$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>Non-assisted</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v> assisted</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$47:$G$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="plus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(Sheet1!$G$42,Sheet1!$C$38)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>22.5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>Non-assisted</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v> assisted</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$48:$G$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="244464216"/>
+        <c:axId val="244459512"/>
+      </c:barChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="244464216"/>
+        <c:axId val="244459512"/>
+      </c:scatterChart>
+      <c:catAx>
+        <c:axId val="244464216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="244459512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="244459512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="244464216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>224628</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>71920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>86591</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>69271</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -362,23 +1543,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,7 +1576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -412,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -430,7 +1611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A9" si="0">A3+1</f>
         <v>3</v>
@@ -448,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -466,7 +1647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -487,7 +1668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -505,7 +1686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -526,7 +1707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -544,7 +1725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -564,7 +1745,465 @@
         <v>6</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>72</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <f>MEDIAN(C13:C17)</f>
+        <v>38</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>50</v>
+      </c>
+      <c r="H13">
+        <f>MEDIAN(G13:G17)</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>35</v>
+      </c>
+      <c r="F14">
+        <v>55</v>
+      </c>
+      <c r="G14">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <v>38</v>
+      </c>
+      <c r="F15">
+        <v>58</v>
+      </c>
+      <c r="G15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>40</v>
+      </c>
+      <c r="C16">
+        <v>40</v>
+      </c>
+      <c r="F16">
+        <v>63</v>
+      </c>
+      <c r="G16">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>42</v>
+      </c>
+      <c r="C17">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>67</v>
+      </c>
+      <c r="G17">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>44</v>
+      </c>
+      <c r="D18">
+        <f xml:space="preserve"> MEDIAN(C21:C25)</f>
+        <v>45</v>
+      </c>
+      <c r="F18">
+        <v>72</v>
+      </c>
+      <c r="H18">
+        <f xml:space="preserve"> MEDIAN(G21:G25)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>45</v>
+      </c>
+      <c r="C19">
+        <f>MEDIAN(B13:B22)</f>
+        <v>43</v>
+      </c>
+      <c r="F19">
+        <v>73</v>
+      </c>
+      <c r="G19">
+        <f>MEDIAN(F13:F22)</f>
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>45</v>
+      </c>
+      <c r="F20">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>50</v>
+      </c>
+      <c r="C21">
+        <v>44</v>
+      </c>
+      <c r="F21">
+        <v>74</v>
+      </c>
+      <c r="G21">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>52</v>
+      </c>
+      <c r="C22">
+        <v>45</v>
+      </c>
+      <c r="F22">
+        <v>107</v>
+      </c>
+      <c r="G22">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>45</v>
+      </c>
+      <c r="G23">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>MEDIAN(B13:B22)</f>
+        <v>43</v>
+      </c>
+      <c r="C24">
+        <v>50</v>
+      </c>
+      <c r="G24">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f>MEDIAN(B13:B22)</f>
+        <v>43</v>
+      </c>
+      <c r="F26">
+        <f>MEDIAN(F13:F22)</f>
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <f>MIN(B13:B22)</f>
+        <v>34</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <f>MIN(G13:G22)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <f>MEDIAN(C13:C17)</f>
+        <v>38</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <f>MEDIAN(G13:G17)</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <f>MEDIAN(B13:B22)</f>
+        <v>43</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <f>MEDIAN(F13:F22)</f>
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <f>MEDIAN(C21:C25)</f>
+        <v>45</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31">
+        <f>MEDIAN(G21:G25)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <f>MAX(B13:B22)</f>
+        <v>52</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32">
+        <f>MAX(F13:F22)</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34">
+        <f>C29-C28</f>
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34">
+        <f>G29-G28</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <f>C29</f>
+        <v>38</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35">
+        <f>G29</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <f>C30-C29</f>
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36">
+        <f>G30-G29</f>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <f>C31-C30</f>
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37">
+        <f>G31-G30</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <f>C32-C31</f>
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38">
+        <f>G32-G31</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39">
+        <f>C31-C29</f>
+        <v>7</v>
+      </c>
+      <c r="F39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39">
+        <f>G31-G29</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40">
+        <f>C39*1.5</f>
+        <v>10.5</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40">
+        <f>G39*1.5</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41">
+        <f>C31+C40</f>
+        <v>55.5</v>
+      </c>
+      <c r="F41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41">
+        <f>G31+G40</f>
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42">
+        <f>G41-G31</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43">
+        <f>G35-G40</f>
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>58</v>
+      </c>
+      <c r="G46">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>11.5</v>
+      </c>
+      <c r="G47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>3.5</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="F13:F22">
+    <sortCondition ref="F13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added box plot results for user study section
</commit_message>
<xml_diff>
--- a/Results/userStudy.xlsx
+++ b/Results/userStudy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Participant Id</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>low lim threshold</t>
+  </si>
+  <si>
+    <t>Mean</t>
   </si>
 </sst>
 </file>
@@ -161,65 +164,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Completion Time  for Sorting Task</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.5837742846879029E-2"/>
+          <c:y val="3.1779049560641322E-2"/>
+          <c:w val="0.8691986497988613"/>
+          <c:h val="0.87776731929362251"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -436,8 +393,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="244464216"/>
-        <c:axId val="244459512"/>
+        <c:axId val="256605608"/>
+        <c:axId val="256606000"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -445,6 +402,9 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:v>Outliers</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -454,14 +414,14 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
-            <c:size val="4"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="FFC000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:srgbClr val="FFC000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -481,6 +441,49 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Mean</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$49:$G$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>69.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -489,11 +492,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="244464216"/>
-        <c:axId val="244459512"/>
+        <c:axId val="256605608"/>
+        <c:axId val="256606000"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="244464216"/>
+        <c:axId val="256605608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -521,7 +524,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -536,7 +539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244459512"/>
+        <c:crossAx val="256606000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -544,7 +547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244459512"/>
+        <c:axId val="256606000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -571,7 +574,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -584,8 +587,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Seconds</a:t>
+                  <a:rPr lang="en-GB" sz="1400" b="1"/>
+                  <a:t>Completion time (Seconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -604,7 +607,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -636,7 +639,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -651,7 +654,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244464216"/>
+        <c:crossAx val="256605608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -663,6 +666,63 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.84501995203743785"/>
+          <c:y val="0.2878023030693263"/>
+          <c:w val="0.10924149894333492"/>
+          <c:h val="0.12766753482806809"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -671,12 +731,9 @@
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1249,16 +1306,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>224628</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>71920</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>69322</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>86591</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>69271</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1543,10 +1600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="D6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,7 +2086,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>13</v>
       </c>
@@ -2045,7 +2102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>8</v>
       </c>
@@ -2061,7 +2118,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>9</v>
       </c>
@@ -2077,7 +2134,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>14</v>
       </c>
@@ -2093,7 +2150,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>15</v>
       </c>
@@ -2109,7 +2166,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>16</v>
       </c>
@@ -2125,7 +2182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>18</v>
       </c>
@@ -2140,8 +2197,12 @@
         <f>G39*1.5</f>
         <v>22.5</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <f>G39*3</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>19</v>
       </c>
@@ -2153,11 +2214,15 @@
         <v>19</v>
       </c>
       <c r="G41">
-        <f>G31+G40</f>
+        <f>$G$31+G40</f>
         <v>95.5</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <f>$G$31+H40</f>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
         <v>21</v>
       </c>
@@ -2166,7 +2231,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>22</v>
       </c>
@@ -2175,7 +2240,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F46">
         <v>58</v>
       </c>
@@ -2183,7 +2248,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F47">
         <v>11.5</v>
       </c>
@@ -2191,12 +2256,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F48">
         <v>3.5</v>
       </c>
       <c r="G48">
         <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>23</v>
+      </c>
+      <c r="F49">
+        <f>AVERAGE(F13:F22)</f>
+        <v>69.2</v>
+      </c>
+      <c r="G49">
+        <f>AVERAGE(B13:B22)</f>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tlx results to thesis
</commit_message>
<xml_diff>
--- a/Results/userStudy.xlsx
+++ b/Results/userStudy.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>Participant Id</t>
   </si>
@@ -97,13 +98,54 @@
   <si>
     <t>Mean</t>
   </si>
+  <si>
+    <t>Mental</t>
+  </si>
+  <si>
+    <t>Temporal</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Effor</t>
+  </si>
+  <si>
+    <t>Frustration</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Assisted</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>TLX</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Participant ID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -131,8 +173,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,8 +439,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="256605608"/>
-        <c:axId val="256606000"/>
+        <c:axId val="440763272"/>
+        <c:axId val="440763664"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -492,11 +538,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="256605608"/>
-        <c:axId val="256606000"/>
+        <c:axId val="440763272"/>
+        <c:axId val="440763664"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="256605608"/>
+        <c:axId val="440763272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,7 +585,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256606000"/>
+        <c:crossAx val="440763664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -547,7 +593,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256606000"/>
+        <c:axId val="440763664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +700,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256605608"/>
+        <c:crossAx val="440763272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -734,6 +780,868 @@
     <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.535170917829274E-2"/>
+          <c:y val="0.12195641660030013"/>
+          <c:w val="0.75565459272780922"/>
+          <c:h val="0.72654870510161074"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Assisted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Non-Assisted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="90"/>
+        <c:axId val="493719904"/>
+        <c:axId val="493719512"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="493719904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600" b="1"/>
+                  <a:t>Participant</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600" b="1" baseline="0"/>
+                  <a:t> ID</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1600" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.36625314782325369"/>
+              <c:y val="0.91276614363963438"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="493719512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="493719512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600" b="1"/>
+                  <a:t>Score (out of 6)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="493719904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.83304156228066661"/>
+          <c:y val="0.41183692575681158"/>
+          <c:w val="0.1651116196613385"/>
+          <c:h val="0.18701228359243038"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1126403347901327"/>
+          <c:y val="6.1822849066943554E-2"/>
+          <c:w val="0.87085397639315953"/>
+          <c:h val="0.7868218395777451"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Assisted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>Mental</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Temporal</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Performance</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Effort</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Frustration</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Physical</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$M$2:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Non-Assisted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>Mental</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Temporal</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Performance</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Effort</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Frustration</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Physical</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$M$9:$M$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="90"/>
+        <c:axId val="488032560"/>
+        <c:axId val="488032168"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="488032560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488032168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="488032168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
+                  <a:t>TLX Score (out of 100)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488032560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -797,6 +1705,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -1270,6 +2258,1012 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1307,19 +3301,84 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>69322</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>21697</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>214311</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1600,10 +3659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,9 +3673,10 @@
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1632,8 +3692,15 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1649,8 +3716,19 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f xml:space="preserve"> 6- D2</f>
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <f xml:space="preserve"> 6- E2</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1667,8 +3745,20 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f>J2+1</f>
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <f xml:space="preserve"> 6- D3</f>
+        <v>6</v>
+      </c>
+      <c r="L3">
+        <f xml:space="preserve"> 6- E3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A9" si="0">A3+1</f>
         <v>3</v>
@@ -1685,8 +3775,20 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f t="shared" ref="J4:J9" si="1">J3+1</f>
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f xml:space="preserve"> 6- D4</f>
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <f xml:space="preserve"> 6- E4</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1703,8 +3805,20 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <f xml:space="preserve"> 6- D5</f>
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <f xml:space="preserve"> 6- E5</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1724,8 +3838,20 @@
       <c r="F6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <f xml:space="preserve"> 6- D6</f>
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <f xml:space="preserve"> 6- E6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1742,8 +3868,20 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <f xml:space="preserve"> 6- D7</f>
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <f xml:space="preserve"> 6- E7</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1763,8 +3901,20 @@
       <c r="F8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <f xml:space="preserve"> 6- D8</f>
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <f xml:space="preserve"> 6- E8</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1781,8 +3931,20 @@
       <c r="E9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <f xml:space="preserve"> 6- D9</f>
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <f xml:space="preserve"> 6- E9</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1801,8 +3963,19 @@
       <c r="F10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <f xml:space="preserve"> 6- D10</f>
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <f xml:space="preserve"> 6- E10</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1818,8 +3991,19 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <f xml:space="preserve"> 6- D11</f>
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <f xml:space="preserve"> 6- E11</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>34</v>
       </c>
@@ -1841,7 +4025,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>35</v>
       </c>
@@ -1855,7 +4039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>38</v>
       </c>
@@ -1869,7 +4053,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>40</v>
       </c>
@@ -2281,6 +4465,555 @@
   <sortState ref="F13:F22">
     <sortCondition ref="F13"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1">
+        <f>AVERAGE(B2:K2)</f>
+        <v>4.8</v>
+      </c>
+      <c r="M2">
+        <f>L2*5</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L7" si="0">AVERAGE(B3:K3)</f>
+        <v>7</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M7" si="1">L3*5</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>14</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="0"/>
+        <v>6.3</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>19</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>18</v>
+      </c>
+      <c r="I9">
+        <v>15</v>
+      </c>
+      <c r="J9">
+        <v>18</v>
+      </c>
+      <c r="K9">
+        <v>17</v>
+      </c>
+      <c r="L9" s="1">
+        <f>AVERAGE(B9:K9)</f>
+        <v>17</v>
+      </c>
+      <c r="M9">
+        <f>L9*5</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <v>17</v>
+      </c>
+      <c r="I10">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>17</v>
+      </c>
+      <c r="K10">
+        <v>11</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" ref="L10:L14" si="2">AVERAGE(B10:K10)</f>
+        <v>14</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10:M14" si="3">L10*5</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>13</v>
+      </c>
+      <c r="J11">
+        <v>19</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>17</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <v>13</v>
+      </c>
+      <c r="I12">
+        <v>16</v>
+      </c>
+      <c r="J12">
+        <v>18</v>
+      </c>
+      <c r="K12">
+        <v>15</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="2"/>
+        <v>14.9</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <v>17</v>
+      </c>
+      <c r="I13">
+        <v>15</v>
+      </c>
+      <c r="J13">
+        <v>19</v>
+      </c>
+      <c r="K13">
+        <v>11</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="2"/>
+        <v>12.9</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>9</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>14</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="2"/>
+        <v>6.5</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>32.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
need to add t test to results
</commit_message>
<xml_diff>
--- a/Results/userStudy.xlsx
+++ b/Results/userStudy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,8 +439,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="440763272"/>
-        <c:axId val="440763664"/>
+        <c:axId val="414763152"/>
+        <c:axId val="414763544"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -538,11 +538,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="440763272"/>
-        <c:axId val="440763664"/>
+        <c:axId val="414763152"/>
+        <c:axId val="414763544"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="440763272"/>
+        <c:axId val="414763152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,7 +585,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440763664"/>
+        <c:crossAx val="414763544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -593,7 +593,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="440763664"/>
+        <c:axId val="414763544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,7 +700,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440763272"/>
+        <c:crossAx val="414763152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -957,11 +957,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="90"/>
-        <c:axId val="493719904"/>
-        <c:axId val="493719512"/>
+        <c:axId val="417622824"/>
+        <c:axId val="417623216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="493719904"/>
+        <c:axId val="417622824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493719512"/>
+        <c:crossAx val="417623216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1079,7 +1079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="493719512"/>
+        <c:axId val="417623216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1187,7 +1187,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493719904"/>
+        <c:crossAx val="417622824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1453,11 +1453,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="90"/>
-        <c:axId val="488032560"/>
-        <c:axId val="488032168"/>
+        <c:axId val="417624000"/>
+        <c:axId val="417624392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="488032560"/>
+        <c:axId val="417624000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1500,7 +1500,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488032168"/>
+        <c:crossAx val="417624392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1508,7 +1508,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="488032168"/>
+        <c:axId val="417624392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1555,7 +1555,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1616,7 +1615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488032560"/>
+        <c:crossAx val="417624000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3661,7 +3660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
@@ -3720,11 +3719,11 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <f xml:space="preserve"> 6- D2</f>
+        <f t="shared" ref="K2:K11" si="0" xml:space="preserve"> 6- D2</f>
         <v>6</v>
       </c>
       <c r="L2">
-        <f xml:space="preserve"> 6- E2</f>
+        <f t="shared" ref="L2:L11" si="1" xml:space="preserve"> 6- E2</f>
         <v>6</v>
       </c>
     </row>
@@ -3750,17 +3749,17 @@
         <v>2</v>
       </c>
       <c r="K3">
-        <f xml:space="preserve"> 6- D3</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L3">
-        <f xml:space="preserve"> 6- E3</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A9" si="0">A3+1</f>
+        <f t="shared" ref="A4:A9" si="2">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4">
@@ -3776,21 +3775,21 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J9" si="1">J3+1</f>
+        <f t="shared" ref="J4:J9" si="3">J3+1</f>
         <v>3</v>
       </c>
       <c r="K4">
-        <f xml:space="preserve"> 6- D4</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L4">
-        <f xml:space="preserve"> 6- E4</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B5">
@@ -3806,84 +3805,84 @@
         <v>0</v>
       </c>
       <c r="J5">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K5">
-        <f xml:space="preserve"> 6- D5</f>
-        <v>6</v>
-      </c>
-      <c r="L5">
-        <f xml:space="preserve"> 6- E5</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>35</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="K6">
-        <f xml:space="preserve"> 6- D6</f>
-        <v>6</v>
-      </c>
-      <c r="L6">
-        <f xml:space="preserve"> 6- E6</f>
-        <v>4</v>
-      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>73</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>45</v>
-      </c>
-      <c r="C7">
-        <v>73</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="J7">
+      <c r="L7">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K7">
-        <f xml:space="preserve"> 6- D7</f>
-        <v>6</v>
-      </c>
-      <c r="L7">
-        <f xml:space="preserve"> 6- E7</f>
-        <v>6</v>
-      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B8">
@@ -3902,21 +3901,21 @@
         <v>5</v>
       </c>
       <c r="J8">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="K8">
-        <f xml:space="preserve"> 6- D8</f>
-        <v>6</v>
-      </c>
-      <c r="L8">
-        <f xml:space="preserve"> 6- E8</f>
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B9">
@@ -3932,15 +3931,15 @@
         <v>3</v>
       </c>
       <c r="J9">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="K9">
-        <f xml:space="preserve"> 6- D9</f>
-        <v>6</v>
-      </c>
-      <c r="L9">
-        <f xml:space="preserve"> 6- E9</f>
         <v>3</v>
       </c>
     </row>
@@ -3967,11 +3966,11 @@
         <v>9</v>
       </c>
       <c r="K10">
-        <f xml:space="preserve"> 6- D10</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L10">
-        <f xml:space="preserve"> 6- E10</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -3995,11 +3994,11 @@
         <v>10</v>
       </c>
       <c r="K11">
-        <f xml:space="preserve"> 6- D11</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L11">
-        <f xml:space="preserve"> 6- E11</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -4475,10 +4474,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4486,7 +4485,7 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>30</v>
       </c>
@@ -4497,7 +4496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -4540,7 +4539,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -4583,7 +4582,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -4626,7 +4625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -4669,7 +4668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4712,7 +4711,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -4755,7 +4754,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -4797,8 +4796,16 @@
         <f>L9*5</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <f>M9-M2</f>
+        <v>61</v>
+      </c>
+      <c r="P9">
+        <f>M13-M6</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -4841,7 +4848,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -4884,7 +4891,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -4927,7 +4934,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -4970,7 +4977,7 @@
         <v>64.5</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
added t test results
</commit_message>
<xml_diff>
--- a/Results/userStudy.xlsx
+++ b/Results/userStudy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>Participant Id</t>
   </si>
@@ -131,6 +131,42 @@
   <si>
     <t>Participant ID</t>
   </si>
+  <si>
+    <t>t test</t>
+  </si>
+  <si>
+    <t>mean assisted</t>
+  </si>
+  <si>
+    <t>mean nonassisted</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>variability of groups</t>
+  </si>
+  <si>
+    <t>variance asssited</t>
+  </si>
+  <si>
+    <t>variance non-assisted</t>
+  </si>
+  <si>
+    <t>variance over N assisted</t>
+  </si>
+  <si>
+    <t>variance over N nonassisted</t>
+  </si>
+  <si>
+    <t>sum of variance over N</t>
+  </si>
+  <si>
+    <t>root of sum</t>
+  </si>
+  <si>
+    <t>t value</t>
+  </si>
 </sst>
 </file>
 
@@ -173,10 +209,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -439,8 +478,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="414763152"/>
-        <c:axId val="414763544"/>
+        <c:axId val="457408312"/>
+        <c:axId val="457409096"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -538,11 +577,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="414763152"/>
-        <c:axId val="414763544"/>
+        <c:axId val="457408312"/>
+        <c:axId val="457409096"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="414763152"/>
+        <c:axId val="457408312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,7 +624,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414763544"/>
+        <c:crossAx val="457409096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -593,7 +632,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="414763544"/>
+        <c:axId val="457409096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,7 +739,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414763152"/>
+        <c:crossAx val="457408312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -957,11 +996,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="90"/>
-        <c:axId val="417622824"/>
-        <c:axId val="417623216"/>
+        <c:axId val="457410272"/>
+        <c:axId val="457410664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="417622824"/>
+        <c:axId val="457410272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1110,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417623216"/>
+        <c:crossAx val="457410664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1079,7 +1118,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="417623216"/>
+        <c:axId val="457410664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1187,7 +1226,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417622824"/>
+        <c:crossAx val="457410272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1453,11 +1492,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="90"/>
-        <c:axId val="417624000"/>
-        <c:axId val="417624392"/>
+        <c:axId val="457411840"/>
+        <c:axId val="457412232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="417624000"/>
+        <c:axId val="457411840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1500,7 +1539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417624392"/>
+        <c:crossAx val="457412232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1508,7 +1547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="417624392"/>
+        <c:axId val="457412232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1615,7 +1654,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417624000"/>
+        <c:crossAx val="457411840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3658,10 +3697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3673,6 +3712,7 @@
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4269,7 +4309,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>13</v>
       </c>
@@ -4285,7 +4325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>8</v>
       </c>
@@ -4301,7 +4341,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>9</v>
       </c>
@@ -4317,7 +4357,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>14</v>
       </c>
@@ -4333,7 +4373,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>15</v>
       </c>
@@ -4349,7 +4389,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>16</v>
       </c>
@@ -4365,7 +4405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>18</v>
       </c>
@@ -4385,7 +4425,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>19</v>
       </c>
@@ -4405,7 +4445,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
         <v>21</v>
       </c>
@@ -4414,7 +4454,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>22</v>
       </c>
@@ -4423,7 +4463,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="F46">
         <v>58</v>
       </c>
@@ -4431,23 +4471,66 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="F47">
         <v>11.5</v>
       </c>
       <c r="G47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K47" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="P47">
+        <v>50</v>
+      </c>
+      <c r="Q47">
+        <f>P47-$L$48</f>
+        <v>7.5</v>
+      </c>
+      <c r="S47">
+        <f>Q47^2</f>
+        <v>56.25</v>
+      </c>
+      <c r="U47">
+        <f>_xlfn.VAR.P(P47:P56)</f>
+        <v>31.65</v>
+      </c>
+    </row>
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="F48">
         <v>3.5</v>
       </c>
       <c r="G48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>36</v>
+      </c>
+      <c r="L48">
+        <f>AVERAGE(B2:B11)</f>
+        <v>42.5</v>
+      </c>
+      <c r="P48">
+        <v>44</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" ref="Q48:Q56" si="4">P48-$L$48</f>
+        <v>1.5</v>
+      </c>
+      <c r="S48">
+        <f t="shared" ref="S48:S56" si="5">Q48^2</f>
+        <v>2.25</v>
+      </c>
+      <c r="V48">
+        <f>U47*(10/9)</f>
+        <v>35.166666666666664</v>
+      </c>
+    </row>
+    <row r="49" spans="5:22" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
         <v>23</v>
       </c>
@@ -4458,14 +4541,210 @@
       <c r="G49">
         <f>AVERAGE(B13:B22)</f>
         <v>42.5</v>
+      </c>
+      <c r="K49" t="s">
+        <v>37</v>
+      </c>
+      <c r="L49">
+        <f>AVERAGE(C2:C11)</f>
+        <v>69.2</v>
+      </c>
+      <c r="P49">
+        <v>52</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="4"/>
+        <v>9.5</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="5"/>
+        <v>90.25</v>
+      </c>
+    </row>
+    <row r="50" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>38</v>
+      </c>
+      <c r="L50">
+        <f>L49-L48</f>
+        <v>26.700000000000003</v>
+      </c>
+      <c r="P50">
+        <v>38</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="4"/>
+        <v>-4.5</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="5"/>
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="51" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="P51">
+        <v>35</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="4"/>
+        <v>-7.5</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="5"/>
+        <v>56.25</v>
+      </c>
+    </row>
+    <row r="52" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="P52">
+        <v>45</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="5"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="53" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="K53" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="P53">
+        <v>42</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="4"/>
+        <v>-0.5</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="54" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="K54" t="s">
+        <v>40</v>
+      </c>
+      <c r="L54">
+        <f>_xlfn.VAR.P(B2:B11) *COUNT(B2:B11) / (COUNT(B2:B11) - 1)</f>
+        <v>35.166666666666664</v>
+      </c>
+      <c r="P54">
+        <v>34</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="4"/>
+        <v>-8.5</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="5"/>
+        <v>72.25</v>
+      </c>
+      <c r="U54">
+        <f>_xlfn.VAR.P(C2:C11)</f>
+        <v>222.76</v>
+      </c>
+      <c r="V54">
+        <f>U54*10/9</f>
+        <v>247.51111111111109</v>
+      </c>
+    </row>
+    <row r="55" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="K55" t="s">
+        <v>41</v>
+      </c>
+      <c r="L55">
+        <f>_xlfn.VAR.P(C2:C11) *COUNT(C2:C11) / (COUNT(C2:C11) - 1)</f>
+        <v>247.51111111111109</v>
+      </c>
+      <c r="P55">
+        <v>40</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="4"/>
+        <v>-2.5</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="5"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="56" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="K56" t="s">
+        <v>42</v>
+      </c>
+      <c r="L56">
+        <f>L54/COUNT(B2:B11)</f>
+        <v>3.5166666666666666</v>
+      </c>
+      <c r="P56">
+        <v>45</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="5"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="57" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="K57" t="s">
+        <v>43</v>
+      </c>
+      <c r="L57">
+        <f>L55/COUNT(C2:C11)</f>
+        <v>24.751111111111108</v>
+      </c>
+    </row>
+    <row r="58" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="K58" t="s">
+        <v>44</v>
+      </c>
+      <c r="L58">
+        <f>L57+L56</f>
+        <v>28.267777777777773</v>
+      </c>
+      <c r="S58">
+        <f>SUM(S47:S56)</f>
+        <v>316.5</v>
+      </c>
+      <c r="T58">
+        <f>S58/10</f>
+        <v>31.65</v>
+      </c>
+    </row>
+    <row r="59" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
+        <v>45</v>
+      </c>
+      <c r="L59">
+        <f>SQRT(L58)</f>
+        <v>5.3167450359950283</v>
+      </c>
+    </row>
+    <row r="61" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="K61" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L61" s="1">
+        <f>L50/L59</f>
+        <v>5.0218695497409911</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="F13:F22">
     <sortCondition ref="F13"/>
   </sortState>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="K53:M53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4476,7 +4755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added t test values to tlx, box plot for error
</commit_message>
<xml_diff>
--- a/Results/userStudy.xlsx
+++ b/Results/userStudy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>Participant Id</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>t value</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Combined TLX</t>
   </si>
 </sst>
 </file>
@@ -478,8 +484,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="457408312"/>
-        <c:axId val="457409096"/>
+        <c:axId val="568644048"/>
+        <c:axId val="568644440"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -577,11 +583,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="457408312"/>
-        <c:axId val="457409096"/>
+        <c:axId val="568644048"/>
+        <c:axId val="568644440"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="457408312"/>
+        <c:axId val="568644048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -624,7 +630,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457409096"/>
+        <c:crossAx val="568644440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -632,7 +638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457409096"/>
+        <c:axId val="568644440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,7 +745,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457408312"/>
+        <c:crossAx val="568644048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -996,11 +1002,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="90"/>
-        <c:axId val="457410272"/>
-        <c:axId val="457410664"/>
+        <c:axId val="574109808"/>
+        <c:axId val="572821912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457410272"/>
+        <c:axId val="574109808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,7 +1116,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457410664"/>
+        <c:crossAx val="572821912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1118,7 +1124,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457410664"/>
+        <c:axId val="572821912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1226,7 +1232,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457410272"/>
+        <c:crossAx val="574109808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1319,6 +1325,777 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="579108000"/>
+        <c:axId val="570841160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="579108000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="570841160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="570841160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="579108000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Non-assisted</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Non-assisted</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="plus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$K$38</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Non-assisted</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="579765056"/>
+        <c:axId val="579341728"/>
+      </c:barChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Mean</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="579765056"/>
+        <c:axId val="579341728"/>
+      </c:scatterChart>
+      <c:catAx>
+        <c:axId val="579765056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="579341728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="579341728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" b="1"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" b="1" baseline="0"/>
+                  <a:t> of Errors</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1400" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="579765056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1457,7 +2234,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$M$9:$M$14</c:f>
+              <c:f>Sheet2!$M$11:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1492,11 +2269,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="90"/>
-        <c:axId val="457411840"/>
-        <c:axId val="457412232"/>
+        <c:axId val="572822696"/>
+        <c:axId val="572823088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457411840"/>
+        <c:axId val="572822696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1539,7 +2316,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457412232"/>
+        <c:crossAx val="572823088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1547,7 +2324,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457412232"/>
+        <c:axId val="572823088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1594,6 +2371,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1654,7 +2432,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457411840"/>
+        <c:crossAx val="572822696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1823,6 +2601,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -2832,7 +3690,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3036,6 +3894,1016 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -3338,16 +5206,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>21697</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>870696</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>55315</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>473448</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>43143</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3368,16 +5236,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>214311</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>561694</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>180134</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>170888</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>42022</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3396,6 +5264,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>33617</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>135590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1086970</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>21290</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>169209</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>156883</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3404,15 +5332,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>276224</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3699,8 +5627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="D6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z30" sqref="Z30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4105,8 +6033,11 @@
       <c r="G16">
         <v>63</v>
       </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>42</v>
       </c>
@@ -4119,8 +6050,11 @@
       <c r="G17">
         <v>67</v>
       </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>44</v>
       </c>
@@ -4135,8 +6069,11 @@
         <f xml:space="preserve"> MEDIAN(G21:G25)</f>
         <v>73</v>
       </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>45</v>
       </c>
@@ -4151,16 +6088,22 @@
         <f>MEDIAN(F13:F22)</f>
         <v>69.5</v>
       </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>45</v>
       </c>
       <c r="F20">
         <v>73</v>
       </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>50</v>
       </c>
@@ -4173,8 +6116,12 @@
       <c r="G21">
         <v>72</v>
       </c>
+      <c r="M21">
+        <f>MEDIAN(L16:L26)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>52</v>
       </c>
@@ -4187,16 +6134,22 @@
       <c r="G22">
         <v>73</v>
       </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>45</v>
       </c>
       <c r="G23">
         <v>73</v>
       </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24">
         <f>MEDIAN(B13:B22)</f>
         <v>43</v>
@@ -4207,8 +6160,11 @@
       <c r="G24">
         <v>74</v>
       </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>52</v>
       </c>
@@ -4218,8 +6174,11 @@
       <c r="G25">
         <v>107</v>
       </c>
+      <c r="L25">
+        <v>3</v>
+      </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26">
         <f>MEDIAN(B13:B22)</f>
         <v>43</v>
@@ -4228,8 +6187,11 @@
         <f>MEDIAN(F13:F22)</f>
         <v>69.5</v>
       </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>7</v>
       </c>
@@ -4244,8 +6206,15 @@
         <f>MIN(G13:G22)</f>
         <v>50</v>
       </c>
+      <c r="J28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28">
+        <f>MIN(L16)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>8</v>
       </c>
@@ -4260,8 +6229,14 @@
         <f>MEDIAN(G13:G17)</f>
         <v>58</v>
       </c>
+      <c r="J29" t="s">
+        <v>8</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>10</v>
       </c>
@@ -4276,8 +6251,14 @@
         <f>MEDIAN(F13:F22)</f>
         <v>69.5</v>
       </c>
+      <c r="J30" t="s">
+        <v>10</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>11</v>
       </c>
@@ -4292,8 +6273,15 @@
         <f>MEDIAN(G21:G25)</f>
         <v>73</v>
       </c>
+      <c r="J31" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31">
+        <f>MEDIAN(L22:L26)</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>12</v>
       </c>
@@ -4307,6 +6295,13 @@
       <c r="G32">
         <f>MAX(F13:F22)</f>
         <v>107</v>
+      </c>
+      <c r="J32" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32">
+        <f>MAX(L22:L26)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.25">
@@ -4324,6 +6319,13 @@
         <f>G29-G28</f>
         <v>8</v>
       </c>
+      <c r="J34" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34">
+        <f>K29-K28</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -4340,6 +6342,13 @@
         <f>G29</f>
         <v>58</v>
       </c>
+      <c r="J35" t="s">
+        <v>8</v>
+      </c>
+      <c r="K35">
+        <f>K29</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
@@ -4356,6 +6365,12 @@
         <f>G30-G29</f>
         <v>11.5</v>
       </c>
+      <c r="J36" t="s">
+        <v>9</v>
+      </c>
+      <c r="K36">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -4372,6 +6387,13 @@
         <f>G31-G30</f>
         <v>3.5</v>
       </c>
+      <c r="J37" t="s">
+        <v>14</v>
+      </c>
+      <c r="K37">
+        <f>K31-K30</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -4388,6 +6410,13 @@
         <f>G32-G31</f>
         <v>34</v>
       </c>
+      <c r="J38" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38">
+        <f>K32-K31</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -4404,6 +6433,13 @@
         <f>G31-G29</f>
         <v>15</v>
       </c>
+      <c r="J39" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39">
+        <f>K31-K29</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
@@ -4424,6 +6460,9 @@
         <f>G39*3</f>
         <v>45</v>
       </c>
+      <c r="J40" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
@@ -4443,6 +6482,13 @@
       <c r="H41">
         <f>$G$31+H40</f>
         <v>118</v>
+      </c>
+      <c r="J41" t="s">
+        <v>47</v>
+      </c>
+      <c r="K41">
+        <f>AVERAGE(E2:E11)</f>
+        <v>0.8</v>
       </c>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.25">
@@ -4738,8 +6784,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="F13:F22">
-    <sortCondition ref="F13"/>
+  <sortState ref="L16:L25">
+    <sortCondition ref="L18"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="K1:L1"/>
@@ -4753,15 +6799,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -5033,270 +7079,444 @@
         <v>31.5</v>
       </c>
     </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B2:B7)</f>
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:K8" si="2">SUM(C2:C7)</f>
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
       <c r="B9">
-        <v>17</v>
+        <f>B8*5</f>
+        <v>225</v>
       </c>
       <c r="C9">
-        <v>17</v>
+        <f t="shared" ref="C9:K9" si="3">C8*5</f>
+        <v>115</v>
       </c>
       <c r="D9">
-        <v>16</v>
+        <f t="shared" si="3"/>
+        <v>230</v>
       </c>
       <c r="E9">
-        <v>18</v>
+        <f t="shared" si="3"/>
+        <v>95</v>
       </c>
       <c r="F9">
-        <v>19</v>
+        <f t="shared" si="3"/>
+        <v>70</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>145</v>
       </c>
       <c r="H9">
-        <v>18</v>
+        <f t="shared" si="3"/>
+        <v>150</v>
       </c>
       <c r="I9">
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>150</v>
       </c>
       <c r="J9">
-        <v>18</v>
+        <f t="shared" si="3"/>
+        <v>200</v>
       </c>
       <c r="K9">
-        <v>17</v>
-      </c>
-      <c r="L9" s="1">
-        <f>AVERAGE(B9:K9)</f>
-        <v>17</v>
-      </c>
-      <c r="M9">
-        <f>L9*5</f>
-        <v>85</v>
+        <f t="shared" si="3"/>
+        <v>80</v>
       </c>
       <c r="O9">
-        <f>M9-M2</f>
+        <f>M11-M2</f>
         <v>61</v>
       </c>
       <c r="P9">
-        <f>M13-M6</f>
+        <f>M15-M6</f>
         <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>16</v>
-      </c>
-      <c r="E10">
-        <v>15</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>16</v>
-      </c>
-      <c r="H10">
-        <v>17</v>
-      </c>
-      <c r="I10">
-        <v>16</v>
-      </c>
-      <c r="J10">
-        <v>17</v>
-      </c>
-      <c r="K10">
-        <v>11</v>
-      </c>
-      <c r="L10" s="1">
-        <f t="shared" ref="L10:L14" si="2">AVERAGE(B10:K10)</f>
-        <v>14</v>
-      </c>
-      <c r="M10">
-        <f t="shared" ref="M10:M14" si="3">L10*5</f>
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G11">
         <v>15</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="I11">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J11">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K11">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <f>AVERAGE(B11:K11)</f>
+        <v>17</v>
       </c>
       <c r="M11">
-        <f t="shared" si="3"/>
-        <v>40</v>
+        <f>L11*5</f>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12">
         <v>16</v>
       </c>
       <c r="E12">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G12">
         <v>16</v>
       </c>
       <c r="H12">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I12">
         <v>16</v>
       </c>
       <c r="J12">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K12">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="2"/>
-        <v>14.9</v>
+        <f t="shared" ref="L12:L16" si="4">AVERAGE(B12:K12)</f>
+        <v>14</v>
       </c>
       <c r="M12">
-        <f t="shared" si="3"/>
-        <v>74.5</v>
+        <f t="shared" ref="M12:M16" si="5">L12*5</f>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
         <v>15</v>
       </c>
-      <c r="D13">
-        <v>17</v>
-      </c>
-      <c r="E13">
-        <v>6</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>16</v>
-      </c>
       <c r="H13">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="I13">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J13">
         <v>19</v>
       </c>
       <c r="K13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="2"/>
-        <v>12.9</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="M13">
-        <f t="shared" si="3"/>
-        <v>64.5</v>
+        <f t="shared" si="5"/>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>16</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <v>16</v>
+      </c>
+      <c r="J14">
+        <v>18</v>
+      </c>
+      <c r="K14">
+        <v>15</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="4"/>
+        <v>14.9</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="5"/>
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>16</v>
+      </c>
+      <c r="H15">
+        <v>17</v>
+      </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <v>19</v>
+      </c>
+      <c r="K15">
+        <v>11</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="4"/>
+        <v>12.9</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="5"/>
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>5</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>6</v>
       </c>
-      <c r="D14">
+      <c r="D16">
         <v>11</v>
       </c>
-      <c r="E14">
+      <c r="E16">
         <v>2</v>
       </c>
-      <c r="F14">
+      <c r="F16">
         <v>4</v>
       </c>
-      <c r="G14">
+      <c r="G16">
         <v>7</v>
       </c>
-      <c r="H14">
+      <c r="H16">
         <v>9</v>
       </c>
-      <c r="I14">
+      <c r="I16">
         <v>5</v>
       </c>
-      <c r="J14">
+      <c r="J16">
         <v>14</v>
       </c>
-      <c r="K14">
+      <c r="K16">
         <v>2</v>
       </c>
-      <c r="L14" s="1">
-        <f t="shared" si="2"/>
+      <c r="L16" s="1">
+        <f t="shared" si="4"/>
         <v>6.5</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="3"/>
+      <c r="M16">
+        <f t="shared" si="5"/>
         <v>32.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17">
+        <f>SUM(B11:B16)</f>
+        <v>74</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:K17" si="6">SUM(C11:C16)</f>
+        <v>71</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="6"/>
+        <v>78</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="6"/>
+        <v>61</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="6"/>
+        <v>38</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="6"/>
+        <v>85</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="6"/>
+        <v>76</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="6"/>
+        <v>105</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="6"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>B17*5</f>
+        <v>370</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:K18" si="7">C17*5</f>
+        <v>355</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="7"/>
+        <v>390</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="7"/>
+        <v>305</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="7"/>
+        <v>190</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="7"/>
+        <v>425</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="7"/>
+        <v>380</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="7"/>
+        <v>400</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="7"/>
+        <v>525</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="7"/>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
need to proof read
</commit_message>
<xml_diff>
--- a/Results/userStudy.xlsx
+++ b/Results/userStudy.xlsx
@@ -484,8 +484,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="228352120"/>
-        <c:axId val="228352512"/>
+        <c:axId val="235351400"/>
+        <c:axId val="235351792"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -583,11 +583,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228352120"/>
-        <c:axId val="228352512"/>
+        <c:axId val="235351400"/>
+        <c:axId val="235351792"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="228352120"/>
+        <c:axId val="235351400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,7 +630,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228352512"/>
+        <c:crossAx val="235351792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -638,7 +638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228352512"/>
+        <c:axId val="235351792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,7 +745,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228352120"/>
+        <c:crossAx val="235351400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1002,11 +1002,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="90"/>
-        <c:axId val="228353296"/>
-        <c:axId val="228353688"/>
+        <c:axId val="235352968"/>
+        <c:axId val="235353360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="228353296"/>
+        <c:axId val="235352968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1116,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228353688"/>
+        <c:crossAx val="235353360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1124,7 +1124,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228353688"/>
+        <c:axId val="235353360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1232,7 +1232,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228353296"/>
+        <c:crossAx val="235352968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1339,7 +1339,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1464,11 +1463,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="228354864"/>
-        <c:axId val="228355256"/>
+        <c:axId val="235354144"/>
+        <c:axId val="235354536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="228354864"/>
+        <c:axId val="235354144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1511,7 +1510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228355256"/>
+        <c:crossAx val="235354536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1519,7 +1518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228355256"/>
+        <c:axId val="235354536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,7 +1569,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228354864"/>
+        <c:crossAx val="235354144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1584,7 +1583,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1856,8 +1854,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="228356040"/>
-        <c:axId val="228356432"/>
+        <c:axId val="235355320"/>
+        <c:axId val="235355712"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1913,11 +1911,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228356040"/>
-        <c:axId val="228356432"/>
+        <c:axId val="235355320"/>
+        <c:axId val="235355712"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="228356040"/>
+        <c:axId val="235355320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1960,7 +1958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228356432"/>
+        <c:crossAx val="235355712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1968,7 +1966,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228356432"/>
+        <c:axId val="235355712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2080,7 +2078,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228356040"/>
+        <c:crossAx val="235355320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2356,11 +2354,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="90"/>
-        <c:axId val="229043864"/>
-        <c:axId val="229044256"/>
+        <c:axId val="235358064"/>
+        <c:axId val="229144632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="229043864"/>
+        <c:axId val="235358064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2403,7 +2401,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229044256"/>
+        <c:crossAx val="229144632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2411,7 +2409,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="229044256"/>
+        <c:axId val="229144632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2458,7 +2456,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2519,7 +2516,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229043864"/>
+        <c:crossAx val="235358064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5714,8 +5711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>